<commit_message>
Something went wrong in the coef
</commit_message>
<xml_diff>
--- a/圖片的價格.xlsx
+++ b/圖片的價格.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="854" uniqueCount="854">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1020" uniqueCount="1020">
   <si>
     <t>filename</t>
   </si>
@@ -2576,6 +2576,504 @@
   </si>
   <si>
     <t>2023_11_27_45</t>
+  </si>
+  <si>
+    <t>2023_11_28_1</t>
+  </si>
+  <si>
+    <t>2023_11_28_2</t>
+  </si>
+  <si>
+    <t>2023_11_28_3</t>
+  </si>
+  <si>
+    <t>2023_11_28_4</t>
+  </si>
+  <si>
+    <t>2023_11_28_5</t>
+  </si>
+  <si>
+    <t>2023_11_28_6</t>
+  </si>
+  <si>
+    <t>2023_11_28_7</t>
+  </si>
+  <si>
+    <t>2023_11_28_8</t>
+  </si>
+  <si>
+    <t>2023_11_28_9</t>
+  </si>
+  <si>
+    <t>2023_11_28_10</t>
+  </si>
+  <si>
+    <t>2023_11_28_11</t>
+  </si>
+  <si>
+    <t>2023_11_28_12</t>
+  </si>
+  <si>
+    <t>2023_11_28_13</t>
+  </si>
+  <si>
+    <t>2023_11_28_14</t>
+  </si>
+  <si>
+    <t>2023_11_28_15</t>
+  </si>
+  <si>
+    <t>2023_11_28_16</t>
+  </si>
+  <si>
+    <t>2023_11_28_17</t>
+  </si>
+  <si>
+    <t>2023_11_28_18</t>
+  </si>
+  <si>
+    <t>2023_11_28_19</t>
+  </si>
+  <si>
+    <t>2023_11_28_20</t>
+  </si>
+  <si>
+    <t>2023_11_28_21</t>
+  </si>
+  <si>
+    <t>2023_11_28_22</t>
+  </si>
+  <si>
+    <t>2023_11_28_23</t>
+  </si>
+  <si>
+    <t>2023_11_28_24</t>
+  </si>
+  <si>
+    <t>2023_11_28_25</t>
+  </si>
+  <si>
+    <t>2023_11_28_26</t>
+  </si>
+  <si>
+    <t>2023_11_28_27</t>
+  </si>
+  <si>
+    <t>2023_11_28_28</t>
+  </si>
+  <si>
+    <t>2023_11_28_29</t>
+  </si>
+  <si>
+    <t>2023_11_28_30</t>
+  </si>
+  <si>
+    <t>2023_11_28_31</t>
+  </si>
+  <si>
+    <t>2023_11_28_32</t>
+  </si>
+  <si>
+    <t>2023_11_28_33</t>
+  </si>
+  <si>
+    <t>2023_11_28_34</t>
+  </si>
+  <si>
+    <t>2023_11_28_35</t>
+  </si>
+  <si>
+    <t>2023_11_29_1</t>
+  </si>
+  <si>
+    <t>2023_11_29_2</t>
+  </si>
+  <si>
+    <t>2023_11_29_3</t>
+  </si>
+  <si>
+    <t>2023_11_29_4</t>
+  </si>
+  <si>
+    <t>2023_11_29_5</t>
+  </si>
+  <si>
+    <t>2023_11_29_6</t>
+  </si>
+  <si>
+    <t>2023_11_29_7</t>
+  </si>
+  <si>
+    <t>2023_11_29_8</t>
+  </si>
+  <si>
+    <t>2023_11_29_9</t>
+  </si>
+  <si>
+    <t>2023_11_29_10</t>
+  </si>
+  <si>
+    <t>2023_11_29_11</t>
+  </si>
+  <si>
+    <t>2023_11_29_12</t>
+  </si>
+  <si>
+    <t>2023_11_29_13</t>
+  </si>
+  <si>
+    <t>2023_11_29_14</t>
+  </si>
+  <si>
+    <t>2023_11_29_15</t>
+  </si>
+  <si>
+    <t>2023_11_29_16</t>
+  </si>
+  <si>
+    <t>2023_11_29_17</t>
+  </si>
+  <si>
+    <t>2023_11_29_18</t>
+  </si>
+  <si>
+    <t>2023_11_29_19</t>
+  </si>
+  <si>
+    <t>2023_11_29_20</t>
+  </si>
+  <si>
+    <t>2023_11_29_21</t>
+  </si>
+  <si>
+    <t>2023_11_29_22</t>
+  </si>
+  <si>
+    <t>2023_11_29_23</t>
+  </si>
+  <si>
+    <t>2023_11_29_24</t>
+  </si>
+  <si>
+    <t>2023_11_29_25</t>
+  </si>
+  <si>
+    <t>2023_11_29_26</t>
+  </si>
+  <si>
+    <t>2023_11_29_27</t>
+  </si>
+  <si>
+    <t>2023_11_29_28</t>
+  </si>
+  <si>
+    <t>2023_11_29_29</t>
+  </si>
+  <si>
+    <t>2023_11_29_30</t>
+  </si>
+  <si>
+    <t>2023_11_29_31</t>
+  </si>
+  <si>
+    <t>2023_11_29_32</t>
+  </si>
+  <si>
+    <t>2023_11_29_33</t>
+  </si>
+  <si>
+    <t>2023_11_29_34</t>
+  </si>
+  <si>
+    <t>2023_11_29_35</t>
+  </si>
+  <si>
+    <t>2023_11_29_36</t>
+  </si>
+  <si>
+    <t>2023_11_29_37</t>
+  </si>
+  <si>
+    <t>2023_11_29_38</t>
+  </si>
+  <si>
+    <t>2023_11_29_39</t>
+  </si>
+  <si>
+    <t>2023_11_29_40</t>
+  </si>
+  <si>
+    <t>2023_11_29_41</t>
+  </si>
+  <si>
+    <t>2023_11_29_42</t>
+  </si>
+  <si>
+    <t>2023_11_29_43</t>
+  </si>
+  <si>
+    <t>2023_11_29_44</t>
+  </si>
+  <si>
+    <t>2023_11_29_45</t>
+  </si>
+  <si>
+    <t>2023_11_29_46</t>
+  </si>
+  <si>
+    <t>2023_11_29_47</t>
+  </si>
+  <si>
+    <t>2023_11_29_48</t>
+  </si>
+  <si>
+    <t>2023_11_29_49</t>
+  </si>
+  <si>
+    <t>2023_11_29_50</t>
+  </si>
+  <si>
+    <t>2023_11_29_51</t>
+  </si>
+  <si>
+    <t>2023_11_29_52</t>
+  </si>
+  <si>
+    <t>2023_11_29_53</t>
+  </si>
+  <si>
+    <t>2023_11_30_1</t>
+  </si>
+  <si>
+    <t>2023_11_30_2</t>
+  </si>
+  <si>
+    <t>2023_11_30_3</t>
+  </si>
+  <si>
+    <t>2023_11_30_4</t>
+  </si>
+  <si>
+    <t>2023_11_30_5</t>
+  </si>
+  <si>
+    <t>2023_11_30_6</t>
+  </si>
+  <si>
+    <t>2023_11_30_7</t>
+  </si>
+  <si>
+    <t>2023_11_30_8</t>
+  </si>
+  <si>
+    <t>2023_11_30_9</t>
+  </si>
+  <si>
+    <t>2023_11_30_10</t>
+  </si>
+  <si>
+    <t>2023_11_30_11</t>
+  </si>
+  <si>
+    <t>2023_11_30_12</t>
+  </si>
+  <si>
+    <t>2023_11_30_13</t>
+  </si>
+  <si>
+    <t>2023_11_30_14</t>
+  </si>
+  <si>
+    <t>2023_11_30_15</t>
+  </si>
+  <si>
+    <t>2023_11_30_16</t>
+  </si>
+  <si>
+    <t>2023_11_30_17</t>
+  </si>
+  <si>
+    <t>2023_11_30_18</t>
+  </si>
+  <si>
+    <t>2023_11_30_19</t>
+  </si>
+  <si>
+    <t>2023_11_30_20</t>
+  </si>
+  <si>
+    <t>2023_11_30_21</t>
+  </si>
+  <si>
+    <t>2023_11_30_22</t>
+  </si>
+  <si>
+    <t>2023_11_30_23</t>
+  </si>
+  <si>
+    <t>2023_11_30_24</t>
+  </si>
+  <si>
+    <t>2023_11_30_25</t>
+  </si>
+  <si>
+    <t>2023_11_30_26</t>
+  </si>
+  <si>
+    <t>2023_11_30_27</t>
+  </si>
+  <si>
+    <t>2023_11_30_28</t>
+  </si>
+  <si>
+    <t>2023_11_30_29</t>
+  </si>
+  <si>
+    <t>2023_12_1_1</t>
+  </si>
+  <si>
+    <t>2023_12_1_2</t>
+  </si>
+  <si>
+    <t>2023_12_1_3</t>
+  </si>
+  <si>
+    <t>2023_12_1_4</t>
+  </si>
+  <si>
+    <t>2023_12_1_5</t>
+  </si>
+  <si>
+    <t>2023_12_1_6</t>
+  </si>
+  <si>
+    <t>2023_12_1_7</t>
+  </si>
+  <si>
+    <t>2023_12_1_8</t>
+  </si>
+  <si>
+    <t>2023_12_1_9</t>
+  </si>
+  <si>
+    <t>2023_12_1_10</t>
+  </si>
+  <si>
+    <t>2023_12_1_11</t>
+  </si>
+  <si>
+    <t>2023_12_1_12</t>
+  </si>
+  <si>
+    <t>2023_12_1_13</t>
+  </si>
+  <si>
+    <t>2023_12_1_14</t>
+  </si>
+  <si>
+    <t>2023_12_1_15</t>
+  </si>
+  <si>
+    <t>2023_12_1_16</t>
+  </si>
+  <si>
+    <t>2023_12_1_17</t>
+  </si>
+  <si>
+    <t>2023_12_1_18</t>
+  </si>
+  <si>
+    <t>2023_12_1_19</t>
+  </si>
+  <si>
+    <t>2023_12_1_20</t>
+  </si>
+  <si>
+    <t>2023_12_1_21</t>
+  </si>
+  <si>
+    <t>2023_12_1_22</t>
+  </si>
+  <si>
+    <t>2023_12_1_23</t>
+  </si>
+  <si>
+    <t>2023_12_1_24</t>
+  </si>
+  <si>
+    <t>2023_12_1_25</t>
+  </si>
+  <si>
+    <t>2023_12_1_26</t>
+  </si>
+  <si>
+    <t>2023_12_1_27</t>
+  </si>
+  <si>
+    <t>2023_12_1_28</t>
+  </si>
+  <si>
+    <t>2023_12_1_29</t>
+  </si>
+  <si>
+    <t>2023_12_1_30</t>
+  </si>
+  <si>
+    <t>2023_12_1_31</t>
+  </si>
+  <si>
+    <t>2023_12_1_32</t>
+  </si>
+  <si>
+    <t>2023_12_1_33</t>
+  </si>
+  <si>
+    <t>2023_12_1_34</t>
+  </si>
+  <si>
+    <t>2023_12_1_35</t>
+  </si>
+  <si>
+    <t>2023_12_1_36</t>
+  </si>
+  <si>
+    <t>2023_12_1_37</t>
+  </si>
+  <si>
+    <t>2023_12_1_38</t>
+  </si>
+  <si>
+    <t>2023_12_1_39</t>
+  </si>
+  <si>
+    <t>2023_12_1_40</t>
+  </si>
+  <si>
+    <t>2023_12_1_41</t>
+  </si>
+  <si>
+    <t>2023_12_1_42</t>
+  </si>
+  <si>
+    <t>2023_12_1_43</t>
+  </si>
+  <si>
+    <t>2023_12_1_44</t>
+  </si>
+  <si>
+    <t>2023_12_1_45</t>
+  </si>
+  <si>
+    <t>2023_12_1_46</t>
+  </si>
+  <si>
+    <t>2023_12_1_47</t>
+  </si>
+  <si>
+    <t>2023_12_1_48</t>
+  </si>
+  <si>
+    <t>2023_12_1_49</t>
   </si>
 </sst>
 </file>
@@ -3212,7 +3710,7 @@
       </c>
       <c r="E5" s="2">
         <f>COUNTIF(D:D,-10)</f>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" s="1">
         <v>-10.0</v>
@@ -3256,7 +3754,7 @@
       </c>
       <c r="E7" s="2">
         <f>COUNTIF(D:D,0)</f>
-        <v>394</v>
+        <v>422</v>
       </c>
       <c r="F7" s="1">
         <v>0.0</v>
@@ -3278,7 +3776,7 @@
       </c>
       <c r="E8" s="2">
         <f>COUNTIF(D:D,5)</f>
-        <v>143</v>
+        <v>154</v>
       </c>
       <c r="F8" s="1">
         <v>5.0</v>
@@ -3300,7 +3798,7 @@
       </c>
       <c r="E9" s="2">
         <f>COUNTIF(D:D,10)</f>
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="F9" s="1">
         <v>10.0</v>
@@ -3322,7 +3820,7 @@
       </c>
       <c r="E10" s="2">
         <f>COUNTIF(D:D,15)</f>
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F10" s="1">
         <v>15.0</v>
@@ -3513,7 +4011,7 @@
       </c>
       <c r="E19" s="2">
         <f>AVERAGE(D:D)</f>
-        <v>3.522135417</v>
+        <v>3.456334563</v>
       </c>
     </row>
     <row r="20">
@@ -3532,7 +4030,7 @@
       </c>
       <c r="E20" s="2">
         <f>STDEV(D:D)</f>
-        <v>8.304632133</v>
+        <v>8.142639993</v>
       </c>
     </row>
     <row r="21">
@@ -6739,7 +7237,7 @@
         <v>85.0</v>
       </c>
       <c r="D251" s="2">
-        <f t="shared" ref="D251:D806" si="2">B251-C251</f>
+        <f t="shared" ref="D251:D851" si="2">B251-C251</f>
         <v>45</v>
       </c>
     </row>
@@ -14866,11 +15364,11 @@
         <v>100.0</v>
       </c>
       <c r="C793" s="1">
-        <v>95.0</v>
+        <v>100.0</v>
       </c>
       <c r="D793" s="2">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="794">
@@ -15075,6 +15573,13 @@
       <c r="B807" s="1">
         <v>60.0</v>
       </c>
+      <c r="C807" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="D807" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="808">
       <c r="A808" s="1" t="s">
@@ -15083,6 +15588,13 @@
       <c r="B808" s="1">
         <v>75.0</v>
       </c>
+      <c r="C808" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D808" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="809">
       <c r="A809" s="1" t="s">
@@ -15091,6 +15603,13 @@
       <c r="B809" s="1">
         <v>80.0</v>
       </c>
+      <c r="C809" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D809" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="810">
       <c r="A810" s="1" t="s">
@@ -15099,6 +15618,13 @@
       <c r="B810" s="1">
         <v>75.0</v>
       </c>
+      <c r="C810" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D810" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="811">
       <c r="A811" s="1" t="s">
@@ -15107,6 +15633,13 @@
       <c r="B811" s="1">
         <v>75.0</v>
       </c>
+      <c r="C811" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D811" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="812">
       <c r="A812" s="1" t="s">
@@ -15115,6 +15648,13 @@
       <c r="B812" s="1">
         <v>80.0</v>
       </c>
+      <c r="C812" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D812" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="813">
       <c r="A813" s="1" t="s">
@@ -15123,6 +15663,13 @@
       <c r="B813" s="1">
         <v>75.0</v>
       </c>
+      <c r="C813" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D813" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="814">
       <c r="A814" s="1" t="s">
@@ -15131,6 +15678,13 @@
       <c r="B814" s="1">
         <v>75.0</v>
       </c>
+      <c r="C814" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D814" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="815">
       <c r="A815" s="1" t="s">
@@ -15139,6 +15693,13 @@
       <c r="B815" s="1">
         <v>75.0</v>
       </c>
+      <c r="C815" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D815" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="816">
       <c r="A816" s="1" t="s">
@@ -15147,6 +15708,13 @@
       <c r="B816" s="1">
         <v>75.0</v>
       </c>
+      <c r="C816" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="D816" s="2">
+        <f t="shared" si="2"/>
+        <v>-10</v>
+      </c>
     </row>
     <row r="817">
       <c r="A817" s="1" t="s">
@@ -15155,6 +15723,13 @@
       <c r="B817" s="1">
         <v>70.0</v>
       </c>
+      <c r="C817" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="D817" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="818">
       <c r="A818" s="1" t="s">
@@ -15163,6 +15738,13 @@
       <c r="B818" s="1">
         <v>55.0</v>
       </c>
+      <c r="C818" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="D818" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="819">
       <c r="A819" s="1" t="s">
@@ -15171,6 +15753,13 @@
       <c r="B819" s="1">
         <v>75.0</v>
       </c>
+      <c r="C819" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D819" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="820">
       <c r="A820" s="1" t="s">
@@ -15179,6 +15768,13 @@
       <c r="B820" s="1">
         <v>75.0</v>
       </c>
+      <c r="C820" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D820" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="821">
       <c r="A821" s="1" t="s">
@@ -15187,6 +15783,13 @@
       <c r="B821" s="1">
         <v>75.0</v>
       </c>
+      <c r="C821" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D821" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="822">
       <c r="A822" s="1" t="s">
@@ -15195,6 +15798,13 @@
       <c r="B822" s="1">
         <v>75.0</v>
       </c>
+      <c r="C822" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D822" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="823">
       <c r="A823" s="1" t="s">
@@ -15203,6 +15813,13 @@
       <c r="B823" s="1">
         <v>75.0</v>
       </c>
+      <c r="C823" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D823" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="824">
       <c r="A824" s="1" t="s">
@@ -15211,6 +15828,13 @@
       <c r="B824" s="1">
         <v>85.0</v>
       </c>
+      <c r="C824" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="D824" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="825">
       <c r="A825" s="1" t="s">
@@ -15219,6 +15843,13 @@
       <c r="B825" s="1">
         <v>70.0</v>
       </c>
+      <c r="C825" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="D825" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="826">
       <c r="A826" s="1" t="s">
@@ -15227,6 +15858,13 @@
       <c r="B826" s="1">
         <v>75.0</v>
       </c>
+      <c r="C826" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D826" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="827">
       <c r="A827" s="1" t="s">
@@ -15235,6 +15873,13 @@
       <c r="B827" s="1">
         <v>50.0</v>
       </c>
+      <c r="C827" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D827" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="828">
       <c r="A828" s="1" t="s">
@@ -15243,6 +15888,13 @@
       <c r="B828" s="1">
         <v>85.0</v>
       </c>
+      <c r="C828" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D828" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="829">
       <c r="A829" s="1" t="s">
@@ -15251,6 +15903,13 @@
       <c r="B829" s="1">
         <v>80.0</v>
       </c>
+      <c r="C829" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D829" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="830">
       <c r="A830" s="1" t="s">
@@ -15259,6 +15918,13 @@
       <c r="B830" s="1">
         <v>75.0</v>
       </c>
+      <c r="C830" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D830" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="831">
       <c r="A831" s="1" t="s">
@@ -15267,6 +15933,13 @@
       <c r="B831" s="1">
         <v>80.0</v>
       </c>
+      <c r="C831" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D831" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="832">
       <c r="A832" s="1" t="s">
@@ -15275,6 +15948,13 @@
       <c r="B832" s="1">
         <v>75.0</v>
       </c>
+      <c r="C832" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="D832" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="833">
       <c r="A833" s="1" t="s">
@@ -15283,6 +15963,13 @@
       <c r="B833" s="1">
         <v>50.0</v>
       </c>
+      <c r="C833" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D833" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="834">
       <c r="A834" s="1" t="s">
@@ -15291,6 +15978,13 @@
       <c r="B834" s="1">
         <v>75.0</v>
       </c>
+      <c r="C834" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D834" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="835">
       <c r="A835" s="1" t="s">
@@ -15299,6 +15993,13 @@
       <c r="B835" s="1">
         <v>75.0</v>
       </c>
+      <c r="C835" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D835" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="836">
       <c r="A836" s="1" t="s">
@@ -15307,6 +16008,13 @@
       <c r="B836" s="1">
         <v>55.0</v>
       </c>
+      <c r="C836" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="D836" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="837">
       <c r="A837" s="1" t="s">
@@ -15315,6 +16023,13 @@
       <c r="B837" s="1">
         <v>110.0</v>
       </c>
+      <c r="C837" s="1">
+        <v>110.0</v>
+      </c>
+      <c r="D837" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="838">
       <c r="A838" s="1" t="s">
@@ -15323,6 +16038,13 @@
       <c r="B838" s="1">
         <v>90.0</v>
       </c>
+      <c r="C838" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="D838" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="839">
       <c r="A839" s="1" t="s">
@@ -15331,6 +16053,13 @@
       <c r="B839" s="1">
         <v>75.0</v>
       </c>
+      <c r="C839" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D839" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="840">
       <c r="A840" s="1" t="s">
@@ -15339,6 +16068,13 @@
       <c r="B840" s="1">
         <v>110.0</v>
       </c>
+      <c r="C840" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="D840" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="841">
       <c r="A841" s="1" t="s">
@@ -15347,6 +16083,13 @@
       <c r="B841" s="1">
         <v>75.0</v>
       </c>
+      <c r="C841" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D841" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="842">
       <c r="A842" s="1" t="s">
@@ -15355,6 +16098,13 @@
       <c r="B842" s="1">
         <v>70.0</v>
       </c>
+      <c r="C842" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="D842" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="843">
       <c r="A843" s="1" t="s">
@@ -15363,6 +16113,13 @@
       <c r="B843" s="1">
         <v>100.0</v>
       </c>
+      <c r="C843" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="D843" s="2">
+        <f t="shared" si="2"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="844">
       <c r="A844" s="1" t="s">
@@ -15371,6 +16128,13 @@
       <c r="B844" s="1">
         <v>50.0</v>
       </c>
+      <c r="C844" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D844" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="845">
       <c r="A845" s="1" t="s">
@@ -15379,6 +16143,13 @@
       <c r="B845" s="1">
         <v>50.0</v>
       </c>
+      <c r="C845" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D845" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="846">
       <c r="A846" s="1" t="s">
@@ -15387,6 +16158,13 @@
       <c r="B846" s="1">
         <v>70.0</v>
       </c>
+      <c r="C846" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="D846" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="847">
       <c r="A847" s="1" t="s">
@@ -15395,6 +16173,13 @@
       <c r="B847" s="1">
         <v>80.0</v>
       </c>
+      <c r="C847" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D847" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
     </row>
     <row r="848">
       <c r="A848" s="1" t="s">
@@ -15403,6 +16188,13 @@
       <c r="B848" s="1">
         <v>75.0</v>
       </c>
+      <c r="C848" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D848" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="849">
       <c r="A849" s="1" t="s">
@@ -15411,6 +16203,13 @@
       <c r="B849" s="1">
         <v>50.0</v>
       </c>
+      <c r="C849" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="D849" s="2">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="850">
       <c r="A850" s="1" t="s">
@@ -15419,6 +16218,13 @@
       <c r="B850" s="1">
         <v>85.0</v>
       </c>
+      <c r="C850" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="D850" s="2">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
     </row>
     <row r="851">
       <c r="A851" s="1" t="s">
@@ -15426,6 +16232,1839 @@
       </c>
       <c r="B851" s="1">
         <v>70.0</v>
+      </c>
+      <c r="C851" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="D851" s="2">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="852">
+      <c r="A852" s="1" t="s">
+        <v>854</v>
+      </c>
+      <c r="B852" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C852" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="853">
+      <c r="A853" s="1" t="s">
+        <v>855</v>
+      </c>
+      <c r="B853" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="C853" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="854">
+      <c r="A854" s="1" t="s">
+        <v>856</v>
+      </c>
+      <c r="B854" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C854" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="855">
+      <c r="A855" s="1" t="s">
+        <v>857</v>
+      </c>
+      <c r="B855" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C855" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="856">
+      <c r="A856" s="3" t="s">
+        <v>858</v>
+      </c>
+      <c r="B856" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C856" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="857">
+      <c r="A857" s="1" t="s">
+        <v>859</v>
+      </c>
+      <c r="B857" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C857" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="858">
+      <c r="A858" s="1" t="s">
+        <v>860</v>
+      </c>
+      <c r="B858" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C858" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="859">
+      <c r="A859" s="1" t="s">
+        <v>861</v>
+      </c>
+      <c r="B859" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C859" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="860">
+      <c r="A860" s="1" t="s">
+        <v>862</v>
+      </c>
+      <c r="B860" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C860" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="861">
+      <c r="A861" s="1" t="s">
+        <v>863</v>
+      </c>
+      <c r="B861" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C861" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="862">
+      <c r="A862" s="1" t="s">
+        <v>864</v>
+      </c>
+      <c r="B862" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C862" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="863">
+      <c r="A863" s="1" t="s">
+        <v>865</v>
+      </c>
+      <c r="B863" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C863" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="864">
+      <c r="A864" s="1" t="s">
+        <v>866</v>
+      </c>
+      <c r="B864" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C864" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="865">
+      <c r="A865" s="1" t="s">
+        <v>867</v>
+      </c>
+      <c r="B865" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C865" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="866">
+      <c r="A866" s="3" t="s">
+        <v>868</v>
+      </c>
+      <c r="B866" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C866" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="867">
+      <c r="A867" s="1" t="s">
+        <v>869</v>
+      </c>
+      <c r="B867" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C867" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="868">
+      <c r="A868" s="1" t="s">
+        <v>870</v>
+      </c>
+      <c r="B868" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C868" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="869">
+      <c r="A869" s="1" t="s">
+        <v>871</v>
+      </c>
+      <c r="B869" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C869" s="1">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="870">
+      <c r="A870" s="1" t="s">
+        <v>872</v>
+      </c>
+      <c r="B870" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C870" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="871">
+      <c r="A871" s="1" t="s">
+        <v>873</v>
+      </c>
+      <c r="B871" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C871" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="872">
+      <c r="A872" s="1" t="s">
+        <v>874</v>
+      </c>
+      <c r="B872" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C872" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="873">
+      <c r="A873" s="1" t="s">
+        <v>875</v>
+      </c>
+      <c r="B873" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C873" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="874">
+      <c r="A874" s="1" t="s">
+        <v>876</v>
+      </c>
+      <c r="B874" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C874" s="1">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="875">
+      <c r="A875" s="1" t="s">
+        <v>877</v>
+      </c>
+      <c r="B875" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="C875" s="1">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="876">
+      <c r="A876" s="1" t="s">
+        <v>878</v>
+      </c>
+      <c r="B876" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C876" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="877">
+      <c r="A877" s="1" t="s">
+        <v>879</v>
+      </c>
+      <c r="B877" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C877" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="878">
+      <c r="A878" s="1" t="s">
+        <v>880</v>
+      </c>
+      <c r="B878" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C878" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="879">
+      <c r="A879" s="1" t="s">
+        <v>881</v>
+      </c>
+      <c r="B879" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C879" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="880">
+      <c r="A880" s="1" t="s">
+        <v>882</v>
+      </c>
+      <c r="B880" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C880" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="881">
+      <c r="A881" s="1" t="s">
+        <v>883</v>
+      </c>
+      <c r="B881" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C881" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="882">
+      <c r="A882" s="1" t="s">
+        <v>884</v>
+      </c>
+      <c r="B882" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="C882" s="1">
+        <v>110.0</v>
+      </c>
+    </row>
+    <row r="883">
+      <c r="A883" s="1" t="s">
+        <v>885</v>
+      </c>
+      <c r="B883" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C883" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="884">
+      <c r="A884" s="1" t="s">
+        <v>886</v>
+      </c>
+      <c r="B884" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C884" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="885">
+      <c r="A885" s="1" t="s">
+        <v>887</v>
+      </c>
+      <c r="B885" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C885" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="886">
+      <c r="A886" s="1" t="s">
+        <v>888</v>
+      </c>
+      <c r="B886" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C886" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="887">
+      <c r="A887" s="3" t="s">
+        <v>889</v>
+      </c>
+      <c r="B887" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C887" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="888">
+      <c r="A888" s="1" t="s">
+        <v>890</v>
+      </c>
+      <c r="B888" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C888" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="889">
+      <c r="A889" s="1" t="s">
+        <v>891</v>
+      </c>
+      <c r="B889" s="1">
+        <v>45.0</v>
+      </c>
+      <c r="C889" s="1">
+        <v>30.0</v>
+      </c>
+    </row>
+    <row r="890">
+      <c r="A890" s="1" t="s">
+        <v>892</v>
+      </c>
+      <c r="B890" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C890" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="891">
+      <c r="A891" s="1" t="s">
+        <v>893</v>
+      </c>
+      <c r="B891" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C891" s="1">
+        <v>45.0</v>
+      </c>
+    </row>
+    <row r="892">
+      <c r="A892" s="1" t="s">
+        <v>894</v>
+      </c>
+      <c r="B892" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C892" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="893">
+      <c r="A893" s="1" t="s">
+        <v>895</v>
+      </c>
+      <c r="B893" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C893" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="894">
+      <c r="A894" s="1" t="s">
+        <v>896</v>
+      </c>
+      <c r="B894" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C894" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="895">
+      <c r="A895" s="1" t="s">
+        <v>897</v>
+      </c>
+      <c r="B895" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="C895" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="896">
+      <c r="A896" s="1" t="s">
+        <v>898</v>
+      </c>
+      <c r="B896" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C896" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="897">
+      <c r="A897" s="1" t="s">
+        <v>899</v>
+      </c>
+      <c r="B897" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C897" s="1">
+        <v>40.0</v>
+      </c>
+    </row>
+    <row r="898">
+      <c r="A898" s="1" t="s">
+        <v>900</v>
+      </c>
+      <c r="B898" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C898" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="899">
+      <c r="A899" s="1" t="s">
+        <v>901</v>
+      </c>
+      <c r="B899" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C899" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="900">
+      <c r="A900" s="1" t="s">
+        <v>902</v>
+      </c>
+      <c r="B900" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C900" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="901">
+      <c r="A901" s="1" t="s">
+        <v>903</v>
+      </c>
+      <c r="B901" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C901" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="902">
+      <c r="A902" s="1" t="s">
+        <v>904</v>
+      </c>
+      <c r="B902" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="C902" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="903">
+      <c r="A903" s="1" t="s">
+        <v>905</v>
+      </c>
+      <c r="B903" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C903" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="904">
+      <c r="A904" s="1" t="s">
+        <v>906</v>
+      </c>
+      <c r="B904" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C904" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="905">
+      <c r="A905" s="1" t="s">
+        <v>907</v>
+      </c>
+      <c r="B905" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C905" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="906">
+      <c r="A906" s="1" t="s">
+        <v>908</v>
+      </c>
+      <c r="B906" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C906" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="907">
+      <c r="A907" s="1" t="s">
+        <v>909</v>
+      </c>
+      <c r="B907" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C907" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="908">
+      <c r="A908" s="1" t="s">
+        <v>910</v>
+      </c>
+      <c r="B908" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="C908" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="909">
+      <c r="A909" s="1" t="s">
+        <v>911</v>
+      </c>
+      <c r="B909" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C909" s="1">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="910">
+      <c r="A910" s="1" t="s">
+        <v>912</v>
+      </c>
+      <c r="B910" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C910" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="911">
+      <c r="A911" s="1" t="s">
+        <v>913</v>
+      </c>
+      <c r="B911" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C911" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="912">
+      <c r="A912" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B912" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C912" s="1">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="913">
+      <c r="A913" s="1" t="s">
+        <v>915</v>
+      </c>
+      <c r="B913" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C913" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="914">
+      <c r="A914" s="1" t="s">
+        <v>916</v>
+      </c>
+      <c r="B914" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C914" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="915">
+      <c r="A915" s="1" t="s">
+        <v>917</v>
+      </c>
+      <c r="B915" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C915" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="916">
+      <c r="A916" s="1" t="s">
+        <v>918</v>
+      </c>
+      <c r="B916" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="C916" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="917">
+      <c r="A917" s="1" t="s">
+        <v>919</v>
+      </c>
+      <c r="B917" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C917" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="918">
+      <c r="A918" s="1" t="s">
+        <v>920</v>
+      </c>
+      <c r="B918" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="C918" s="1">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="919">
+      <c r="A919" s="1" t="s">
+        <v>921</v>
+      </c>
+      <c r="B919" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C919" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="920">
+      <c r="A920" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="B920" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C920" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="921">
+      <c r="A921" s="1" t="s">
+        <v>923</v>
+      </c>
+      <c r="B921" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C921" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="922">
+      <c r="A922" s="1" t="s">
+        <v>924</v>
+      </c>
+      <c r="B922" s="1">
+        <v>115.0</v>
+      </c>
+      <c r="C922" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="923">
+      <c r="A923" s="1" t="s">
+        <v>925</v>
+      </c>
+      <c r="B923" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C923" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="924">
+      <c r="A924" s="1" t="s">
+        <v>926</v>
+      </c>
+      <c r="B924" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C924" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="925">
+      <c r="A925" s="1" t="s">
+        <v>927</v>
+      </c>
+      <c r="B925" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C925" s="1">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="926">
+      <c r="A926" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B926" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C926" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="927">
+      <c r="A927" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="B927" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C927" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="928">
+      <c r="A928" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="B928" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C928" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="929">
+      <c r="A929" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="B929" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C929" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="930">
+      <c r="A930" s="1" t="s">
+        <v>932</v>
+      </c>
+      <c r="B930" s="1">
+        <v>90.0</v>
+      </c>
+      <c r="C930" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="931">
+      <c r="A931" s="3" t="s">
+        <v>933</v>
+      </c>
+      <c r="B931" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C931" s="1">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="932">
+      <c r="A932" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="B932" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C932" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="933">
+      <c r="A933" s="1" t="s">
+        <v>935</v>
+      </c>
+      <c r="B933" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C933" s="1">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="934">
+      <c r="A934" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="B934" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C934" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="935">
+      <c r="A935" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="B935" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C935" s="1">
+        <v>70.0</v>
+      </c>
+    </row>
+    <row r="936">
+      <c r="A936" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="B936" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C936" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="937">
+      <c r="A937" s="1" t="s">
+        <v>939</v>
+      </c>
+      <c r="B937" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C937" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="938">
+      <c r="A938" s="1" t="s">
+        <v>940</v>
+      </c>
+      <c r="B938" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C938" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="939">
+      <c r="A939" s="1" t="s">
+        <v>941</v>
+      </c>
+      <c r="B939" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C939" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="940">
+      <c r="A940" s="1" t="s">
+        <v>942</v>
+      </c>
+      <c r="B940" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C940" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="941">
+      <c r="A941" s="1" t="s">
+        <v>943</v>
+      </c>
+      <c r="B941" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C941" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="942">
+      <c r="A942" s="1" t="s">
+        <v>944</v>
+      </c>
+      <c r="B942" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C942" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="943">
+      <c r="A943" s="1" t="s">
+        <v>945</v>
+      </c>
+      <c r="B943" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C943" s="1">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="944">
+      <c r="A944" s="1" t="s">
+        <v>946</v>
+      </c>
+      <c r="B944" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C944" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="945">
+      <c r="A945" s="1" t="s">
+        <v>947</v>
+      </c>
+      <c r="B945" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C945" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="946">
+      <c r="A946" s="1" t="s">
+        <v>948</v>
+      </c>
+      <c r="B946" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C946" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="947">
+      <c r="A947" s="1" t="s">
+        <v>949</v>
+      </c>
+      <c r="B947" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C947" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="948">
+      <c r="A948" s="1" t="s">
+        <v>950</v>
+      </c>
+      <c r="B948" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C948" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="949">
+      <c r="A949" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="B949" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C949" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="950">
+      <c r="A950" s="1" t="s">
+        <v>952</v>
+      </c>
+      <c r="B950" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C950" s="1">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="951">
+      <c r="A951" s="1" t="s">
+        <v>953</v>
+      </c>
+      <c r="B951" s="1">
+        <v>185.0</v>
+      </c>
+      <c r="C951" s="1">
+        <v>110.0</v>
+      </c>
+    </row>
+    <row r="952">
+      <c r="A952" s="1" t="s">
+        <v>954</v>
+      </c>
+      <c r="B952" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C952" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="953">
+      <c r="A953" s="1" t="s">
+        <v>955</v>
+      </c>
+      <c r="B953" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C953" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="954">
+      <c r="A954" s="1" t="s">
+        <v>956</v>
+      </c>
+      <c r="B954" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C954" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="955">
+      <c r="A955" s="1" t="s">
+        <v>957</v>
+      </c>
+      <c r="B955" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C955" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="956">
+      <c r="A956" s="1" t="s">
+        <v>958</v>
+      </c>
+      <c r="B956" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C956" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="957">
+      <c r="A957" s="1" t="s">
+        <v>959</v>
+      </c>
+      <c r="B957" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C957" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="958">
+      <c r="A958" s="1" t="s">
+        <v>960</v>
+      </c>
+      <c r="B958" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C958" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="959">
+      <c r="A959" s="1" t="s">
+        <v>961</v>
+      </c>
+      <c r="B959" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C959" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="960">
+      <c r="A960" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="B960" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C960" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="961">
+      <c r="A961" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="B961" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C961" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="962">
+      <c r="A962" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="B962" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="C962" s="1">
+        <v>90.0</v>
+      </c>
+    </row>
+    <row r="963">
+      <c r="A963" s="1" t="s">
+        <v>965</v>
+      </c>
+      <c r="B963" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C963" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="964">
+      <c r="A964" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="B964" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C964" s="1">
+        <v>80.0</v>
+      </c>
+    </row>
+    <row r="965">
+      <c r="A965" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="B965" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C965" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="966">
+      <c r="A966" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="B966" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C966" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="967">
+      <c r="A967" s="1" t="s">
+        <v>969</v>
+      </c>
+      <c r="B967" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C967" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="968">
+      <c r="A968" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="B968" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C968" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="969">
+      <c r="A969" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="B969" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C969" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="970">
+      <c r="A970" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="B970" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="C970" s="1">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="971">
+      <c r="A971" s="1" t="s">
+        <v>973</v>
+      </c>
+      <c r="B971" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C971" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="972">
+      <c r="A972" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="B972" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C972" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="973">
+      <c r="A973" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="B973" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C973" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="974">
+      <c r="A974" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="B974" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C974" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="975">
+      <c r="A975" s="1" t="s">
+        <v>977</v>
+      </c>
+      <c r="B975" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C975" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="976">
+      <c r="A976" s="1" t="s">
+        <v>978</v>
+      </c>
+      <c r="B976" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="C976" s="1">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="977">
+      <c r="A977" s="1" t="s">
+        <v>979</v>
+      </c>
+      <c r="B977" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C977" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="978">
+      <c r="A978" s="1" t="s">
+        <v>980</v>
+      </c>
+      <c r="B978" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C978" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="979">
+      <c r="A979" s="1" t="s">
+        <v>981</v>
+      </c>
+      <c r="B979" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C979" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="980">
+      <c r="A980" s="1" t="s">
+        <v>982</v>
+      </c>
+      <c r="B980" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C980" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="981">
+      <c r="A981" s="1" t="s">
+        <v>983</v>
+      </c>
+      <c r="B981" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C981" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="982">
+      <c r="A982" s="1" t="s">
+        <v>984</v>
+      </c>
+      <c r="B982" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C982" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="983">
+      <c r="A983" s="1" t="s">
+        <v>985</v>
+      </c>
+      <c r="B983" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C983" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="984">
+      <c r="A984" s="1" t="s">
+        <v>986</v>
+      </c>
+      <c r="B984" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C984" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="985">
+      <c r="A985" s="1" t="s">
+        <v>987</v>
+      </c>
+      <c r="B985" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C985" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="986">
+      <c r="A986" s="1" t="s">
+        <v>988</v>
+      </c>
+      <c r="B986" s="1">
+        <v>60.0</v>
+      </c>
+      <c r="C986" s="1">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="987">
+      <c r="A987" s="1" t="s">
+        <v>989</v>
+      </c>
+      <c r="B987" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C987" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="988">
+      <c r="A988" s="1" t="s">
+        <v>990</v>
+      </c>
+      <c r="B988" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C988" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="989">
+      <c r="A989" s="1" t="s">
+        <v>991</v>
+      </c>
+      <c r="B989" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C989" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="990">
+      <c r="A990" s="1" t="s">
+        <v>992</v>
+      </c>
+      <c r="B990" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C990" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="991">
+      <c r="A991" s="1" t="s">
+        <v>993</v>
+      </c>
+      <c r="B991" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C991" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="992">
+      <c r="A992" s="1" t="s">
+        <v>994</v>
+      </c>
+      <c r="B992" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C992" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="993">
+      <c r="A993" s="1" t="s">
+        <v>995</v>
+      </c>
+      <c r="B993" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C993" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="994">
+      <c r="A994" s="1" t="s">
+        <v>996</v>
+      </c>
+      <c r="B994" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C994" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="995">
+      <c r="A995" s="1" t="s">
+        <v>997</v>
+      </c>
+      <c r="B995" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C995" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="996">
+      <c r="A996" s="1" t="s">
+        <v>998</v>
+      </c>
+      <c r="B996" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C996" s="1">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="997">
+      <c r="A997" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="B997" s="1">
+        <v>85.0</v>
+      </c>
+      <c r="C997" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="998">
+      <c r="A998" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="B998" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C998" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="999">
+      <c r="A999" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="B999" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C999" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="1000">
+      <c r="A1000" s="1" t="s">
+        <v>1002</v>
+      </c>
+      <c r="B1000" s="1">
+        <v>70.0</v>
+      </c>
+      <c r="C1000" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="1001">
+      <c r="A1001" s="1" t="s">
+        <v>1003</v>
+      </c>
+      <c r="B1001" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="C1001" s="1">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="1002">
+      <c r="A1002" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="B1002" s="1">
+        <v>95.0</v>
+      </c>
+      <c r="C1002" s="1">
+        <v>85.0</v>
+      </c>
+    </row>
+    <row r="1003">
+      <c r="A1003" s="1" t="s">
+        <v>1005</v>
+      </c>
+      <c r="B1003" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C1003" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="1004">
+      <c r="A1004" s="1" t="s">
+        <v>1006</v>
+      </c>
+      <c r="B1004" s="1">
+        <v>50.0</v>
+      </c>
+      <c r="C1004" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="1005">
+      <c r="A1005" s="1" t="s">
+        <v>1007</v>
+      </c>
+      <c r="B1005" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C1005" s="1">
+        <v>50.0</v>
+      </c>
+    </row>
+    <row r="1006">
+      <c r="A1006" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="B1006" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="C1006" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="1007">
+      <c r="A1007" s="1" t="s">
+        <v>1009</v>
+      </c>
+      <c r="B1007" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C1007" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="1008">
+      <c r="A1008" s="1" t="s">
+        <v>1010</v>
+      </c>
+      <c r="B1008" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C1008" s="1">
+        <v>60.0</v>
+      </c>
+    </row>
+    <row r="1009">
+      <c r="A1009" s="1" t="s">
+        <v>1011</v>
+      </c>
+      <c r="B1009" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C1009" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="1010">
+      <c r="A1010" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="B1010" s="1">
+        <v>65.0</v>
+      </c>
+      <c r="C1010" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="1011">
+      <c r="A1011" s="1" t="s">
+        <v>1013</v>
+      </c>
+      <c r="B1011" s="1">
+        <v>100.0</v>
+      </c>
+      <c r="C1011" s="1">
+        <v>100.0</v>
+      </c>
+    </row>
+    <row r="1012">
+      <c r="A1012" s="1" t="s">
+        <v>1014</v>
+      </c>
+      <c r="B1012" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C1012" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="1013">
+      <c r="A1013" s="1" t="s">
+        <v>1015</v>
+      </c>
+      <c r="B1013" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C1013" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="1014">
+      <c r="A1014" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="B1014" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C1014" s="1">
+        <v>65.0</v>
+      </c>
+    </row>
+    <row r="1015">
+      <c r="A1015" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="B1015" s="1">
+        <v>75.0</v>
+      </c>
+      <c r="C1015" s="1">
+        <v>75.0</v>
+      </c>
+    </row>
+    <row r="1016">
+      <c r="A1016" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="B1016" s="1">
+        <v>55.0</v>
+      </c>
+      <c r="C1016" s="1">
+        <v>55.0</v>
+      </c>
+    </row>
+    <row r="1017">
+      <c r="A1017" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="B1017" s="1">
+        <v>80.0</v>
+      </c>
+      <c r="C1017" s="1">
+        <v>65.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>